<commit_message>
Data Wilayah & Import
</commit_message>
<xml_diff>
--- a/dummy_sampel_palawija.xlsx
+++ b/dummy_sampel_palawija.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ubinan-kediri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC31FC2-1B28-4F3B-B170-F445E77A2CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99776274-D664-4E9E-A168-ECA1EEF03D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8928" xr2:uid="{96A0ABE8-BFC3-43C4-A433-185F1D0DE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{96A0ABE8-BFC3-43C4-A433-185F1D0DE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>jenis_sampel</t>
   </si>
@@ -66,98 +57,137 @@
     <t>Jagung</t>
   </si>
   <si>
-    <t>Jawa Timur</t>
-  </si>
-  <si>
-    <t>Kabupaten Kediri</t>
-  </si>
-  <si>
-    <t>Mojo</t>
-  </si>
-  <si>
     <t>Ngetrep</t>
   </si>
   <si>
-    <t>Ngadi</t>
-  </si>
-  <si>
     <t>SLS Mojo 1</t>
   </si>
   <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.29</t>
+  </si>
+  <si>
+    <t>prop</t>
+  </si>
+  <si>
+    <t>kab</t>
+  </si>
+  <si>
+    <t>nmkab</t>
+  </si>
+  <si>
+    <t>nmkec</t>
+  </si>
+  <si>
+    <t>kec</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>subround</t>
+  </si>
+  <si>
+    <t>nks</t>
+  </si>
+  <si>
+    <t>21010109</t>
+  </si>
+  <si>
+    <t>nama_krt</t>
+  </si>
+  <si>
+    <t>Suparni</t>
+  </si>
+  <si>
+    <t>Suparman</t>
+  </si>
+  <si>
+    <t>Suprapto</t>
+  </si>
+  <si>
+    <t>Supono</t>
+  </si>
+  <si>
+    <t>perkiraan_minggu_panen</t>
+  </si>
+  <si>
+    <t>nmprop</t>
+  </si>
+  <si>
+    <t>JAWA TIMUR</t>
+  </si>
+  <si>
+    <t>KABUPATEN KEDIRI</t>
+  </si>
+  <si>
+    <t>MOJO</t>
+  </si>
+  <si>
+    <t>SEMEN</t>
+  </si>
+  <si>
+    <t>desa_kel</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
     <t>SLS Mojo 2</t>
   </si>
   <si>
-    <t>SLS Mojo 3</t>
-  </si>
-  <si>
-    <t>0.75</t>
-  </si>
-  <si>
-    <t>0.85</t>
-  </si>
-  <si>
-    <t>0.29</t>
-  </si>
-  <si>
-    <t>prop</t>
-  </si>
-  <si>
-    <t>kab</t>
-  </si>
-  <si>
-    <t>nmkab</t>
-  </si>
-  <si>
-    <t>nmkec</t>
-  </si>
-  <si>
-    <t>kec</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
-    <t>020</t>
-  </si>
-  <si>
-    <t>nmdesa</t>
-  </si>
-  <si>
-    <t>subround</t>
-  </si>
-  <si>
-    <t>nks</t>
-  </si>
-  <si>
-    <t>21010109</t>
-  </si>
-  <si>
-    <t>nama_krt</t>
-  </si>
-  <si>
-    <t>Suparni</t>
-  </si>
-  <si>
-    <t>Suparman</t>
-  </si>
-  <si>
-    <t>Suprapto</t>
-  </si>
-  <si>
-    <t>Supono</t>
+    <t>bulan</t>
+  </si>
+  <si>
+    <t>tahun</t>
+  </si>
+  <si>
+    <t>rilis</t>
+  </si>
+  <si>
+    <t>2025-04-23 09:34:59</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>fasetanam</t>
+  </si>
+  <si>
+    <t>SLS Semen 1</t>
+  </si>
+  <si>
+    <t>SLS Semen 2</t>
+  </si>
+  <si>
+    <t>SELOPANGGUNG</t>
+  </si>
+  <si>
+    <t>PUHRUBUH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +199,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF020817"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -193,9 +229,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,20 +552,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5A16A2-3DB7-4FF0-BA8A-6B24262442A6}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" customWidth="1"/>
+    <col min="19" max="19" width="29.28515625" customWidth="1"/>
+    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,28 +581,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
       <c r="J1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -562,19 +611,40 @@
         <v>4</v>
       </c>
       <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -582,49 +652,70 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2">
+        <v>6</v>
+      </c>
+      <c r="N2">
+        <v>2025</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>2</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="S2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="1">
-        <v>2</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>35</v>
+      <c r="U2" s="2">
+        <v>111951135</v>
+      </c>
+      <c r="V2" s="2">
+        <v>-7827135</v>
+      </c>
+      <c r="W2">
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -632,49 +723,70 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <v>2025</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>2</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="1">
-        <v>2</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" t="s">
-        <v>36</v>
+      <c r="S3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="2">
+        <v>111951135</v>
+      </c>
+      <c r="V3" s="2">
+        <v>-7827135</v>
+      </c>
+      <c r="W3">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -682,49 +794,70 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
       <c r="J4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4">
+        <v>50</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4">
+        <v>6</v>
+      </c>
+      <c r="N4">
+        <v>2025</v>
+      </c>
+      <c r="O4">
         <v>2</v>
       </c>
-      <c r="L4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="1">
+      <c r="P4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="1">
         <v>2</v>
       </c>
-      <c r="O4" s="1">
+      <c r="R4" s="1">
         <v>21010110</v>
       </c>
-      <c r="P4" t="s">
-        <v>37</v>
+      <c r="S4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" t="s">
+        <v>30</v>
+      </c>
+      <c r="U4" s="2">
+        <v>111951135</v>
+      </c>
+      <c r="V4" s="2">
+        <v>-7827135</v>
+      </c>
+      <c r="W4">
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -732,49 +865,71 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
       <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5">
+        <v>2025</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5" t="s">
         <v>14</v>
       </c>
-      <c r="K5">
+      <c r="Q5" s="1">
         <v>2</v>
       </c>
-      <c r="L5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="1">
-        <v>2</v>
-      </c>
-      <c r="O5" s="1">
+      <c r="R5" s="1">
         <v>21010110</v>
       </c>
-      <c r="P5" t="s">
-        <v>38</v>
+      <c r="S5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U5" s="2">
+        <v>111951135</v>
+      </c>
+      <c r="V5" s="2">
+        <v>-7827135</v>
+      </c>
+      <c r="W5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>